<commit_message>
montagem de torres removida
</commit_message>
<xml_diff>
--- a/associassoes.xlsx
+++ b/associassoes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\viniciusbarros\OneDrive - unb.br\0Aneel\Previsor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\viniciusbarros\OneDrive - unb.br\0Aneel\Previsor\Previsor_Operacao_Comercial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D237FFA4-86DD-490A-9211-FB11A9F5BA20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FADE14D-AE3A-4F6B-81D1-A1A5273521B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23880" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{74B732AD-59D1-4F24-BB3B-F925A4B539CC}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>bdworgs</t>
   </si>
@@ -158,12 +158,6 @@
   </si>
   <si>
     <t>DatOutorgaUsina</t>
-  </si>
-  <si>
-    <t>DatConclusaoTorresOutorgado</t>
-  </si>
-  <si>
-    <t>DatConclusaoTorresRealizado</t>
   </si>
   <si>
     <t>Num_UG</t>
@@ -616,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89EC3E58-B90E-467A-9F43-003EEA57D1AC}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,17 +747,13 @@
       <c r="A17" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>41</v>
-      </c>
+      <c r="B17" s="6"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>42</v>
-      </c>
+      <c r="B18" s="6"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
@@ -805,12 +795,12 @@
     </row>
     <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>